<commit_message>
Fixed problem in publicaitons
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\yannik\yblei.github.io\markdown_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DBF3B9-4ADD-44DC-B19D-2C9062AB891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D15C89-4176-45FD-BEAF-CFA53EB310CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{5DEEBD5F-D318-40E3-BCEE-FEB4EEB67B08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5DEEBD5F-D318-40E3-BCEE-FEB4EEB67B08}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="2" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>Identifying Out-of-Distribution Samples in Real-Time for Safety-Critical 2D Object Detection with Margin Entropy Loss</t>
   </si>
   <si>
-    <t>ECCV UNCV Workshop 2022 - Extended Abstract</t>
-  </si>
-  <si>
     <t>Convolutional Neural Networks (CNNs) are nowadays often employed in vision-based perception stacks for safetycritical applications such as autonomous driving or Unmanned Aerial Vehicles (UAVs). Due to the safety requirements in those use cases, it is important to know the limitations of the CNN and, thus, to detect Out-of-Distribution (OOD) samples. In this work, we present an approach to enable OOD detection for 2D object detection by employing the margin entropy (ME) loss.</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>https://arxiv.org/pdf/2311.17776.pdf</t>
+  </si>
+  <si>
+    <t>ECCV UNCV Workshop</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,19 +574,19 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -594,22 +594,22 @@
         <v>45207</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>